<commit_message>
fusión componentes vacíos asesorías y colaboraciones
</commit_message>
<xml_diff>
--- a/Para.Ivan_Pagina web.xlsx
+++ b/Para.Ivan_Pagina web.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Journals" sheetId="1" state="visible" r:id="rId2"/>
@@ -3839,7 +3839,7 @@
     <t xml:space="preserve">2005-2008</t>
   </si>
   <si>
-    <t xml:space="preserve">ASESORAMIENTO / COLABORACIONES EN ASESORIAS DE LA ANTIGUA PAGINA</t>
+    <t xml:space="preserve">ASESORAMIENTO SE FUSIONA CON COLABORACIONES DE LA ANTIGUA PAGINA</t>
   </si>
   <si>
     <t xml:space="preserve">Waiting RG request</t>
@@ -4237,7 +4237,7 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5324,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5589,12 +5589,12 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="0" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I15" r:id="rId1" display="https://www.xataka.com/investigacion/como-sangre-azul-cangrejo-herradura-nos-esta-ayudando-a-detectar-bacterias-fuera-tierra"/>
@@ -9169,7 +9169,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9718,7 +9718,7 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizacion del subcomponente reports
</commit_message>
<xml_diff>
--- a/Para.Ivan_Pagina web.xlsx
+++ b/Para.Ivan_Pagina web.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Journals" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
     <sheet name="Supervision" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Docencia" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Proyectos" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Asesoramiento" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="ASESORIAS" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="NO.UTILIZARConf.Posters" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -3839,7 +3839,7 @@
     <t xml:space="preserve">2005-2008</t>
   </si>
   <si>
-    <t xml:space="preserve">ASESORAMIENTO SE FUSIONA CON COLABORACIONES DE LA ANTIGUA PAGINA</t>
+    <t xml:space="preserve">ASESORIAS SE FUSIONA CON COLABORACIONES DE LA ANTIGUA PAGINA</t>
   </si>
   <si>
     <t xml:space="preserve">Waiting RG request</t>
@@ -4236,7 +4236,7 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -5324,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10552,7 +10552,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Componente Congresos y conversion a JSON de Congresos, Divulgacion y Docencia
</commit_message>
<xml_diff>
--- a/Para.Ivan_Pagina web.xlsx
+++ b/Para.Ivan_Pagina web.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Journals" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="710">
   <si>
     <t xml:space="preserve">g</t>
   </si>
@@ -831,10 +831,10 @@
     <t xml:space="preserve">PINGERS, Anexo IV</t>
   </si>
   <si>
-    <t xml:space="preserve">Conference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo</t>
+    <t xml:space="preserve">conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo</t>
   </si>
   <si>
     <t xml:space="preserve">	Pierce, G.J., Gutiérrez, P., Fariñas, A., Fernández, D., Petitguyot, M., Read, F.L., Hernández, A., Saavedra, C., Hernandez-Milian, G., Viñas Diéguez, L., Pérez Fernández, B., Jaquot, S., Méndez, P., López, A. y Cedeira, J.</t>
@@ -2176,6 +2176,9 @@
     <t xml:space="preserve">Workshop</t>
   </si>
   <si>
+    <t xml:space="preserve">Tipo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hernandez-Milian, G. y Lusher, A.</t>
   </si>
   <si>
@@ -3840,6 +3843,9 @@
   </si>
   <si>
     <t xml:space="preserve">ASESORIAS SE FUSIONA CON COLABORACIONES DE LA ANTIGUA PAGINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference</t>
   </si>
   <si>
     <t xml:space="preserve">Waiting RG request</t>
@@ -4236,7 +4242,7 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -5337,19 +5343,19 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -5358,181 +5364,181 @@
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>662</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>660</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>668</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>669</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>2021</v>
@@ -5540,50 +5546,50 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>698</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>696</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>695</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5592,7 +5598,7 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -5643,13 +5649,13 @@
         <v>3</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>163</v>
+        <v>708</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>164</v>
+        <v>394</v>
       </c>
       <c r="J1" s="11"/>
     </row>
@@ -6147,7 +6153,7 @@
     </row>
     <row r="26" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="21" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>261</v>
@@ -7447,8 +7453,8 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H71" activeCellId="0" sqref="H71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7456,6 +7462,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="90.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.11"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8898,42 +8905,42 @@
         <v>5</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>164</v>
+        <v>394</v>
       </c>
       <c r="J1" s="11"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="7" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="7" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>2017</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8941,13 +8948,13 @@
         <v>150</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>2016</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8955,16 +8962,16 @@
         <v>150</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>2014</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8972,13 +8979,13 @@
         <v>150</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>2014</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8986,13 +8993,13 @@
         <v>150</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>2013</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9000,13 +9007,13 @@
         <v>150</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9014,16 +9021,16 @@
         <v>150</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9031,84 +9038,84 @@
         <v>150</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F11" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F12" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F13" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F14" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9116,33 +9123,33 @@
         <v>318</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F15" s="7" t="n">
         <v>2010</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F16" s="7" t="n">
         <v>2010</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -9190,16 +9197,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>164</v>
+        <v>394</v>
       </c>
       <c r="K1" s="11"/>
     </row>
@@ -9208,20 +9215,20 @@
         <v>279</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9229,20 +9236,20 @@
         <v>279</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>2020</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9250,18 +9257,18 @@
         <v>279</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>2020</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9269,20 +9276,20 @@
         <v>279</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>2020</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9290,20 +9297,20 @@
         <v>279</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>2020</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9311,20 +9318,20 @@
         <v>279</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>2019</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9332,18 +9339,18 @@
         <v>279</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9351,16 +9358,16 @@
         <v>279</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -9370,18 +9377,18 @@
         <v>279</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9389,16 +9396,16 @@
         <v>279</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F11" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -9408,16 +9415,16 @@
         <v>279</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F12" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -9427,18 +9434,18 @@
         <v>279</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F13" s="7" t="n">
         <v>2017</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9446,16 +9453,16 @@
         <v>279</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F14" s="7" t="n">
         <v>2017</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -9465,16 +9472,16 @@
         <v>279</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F15" s="7" t="n">
         <v>2008</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -9484,16 +9491,16 @@
         <v>279</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F16" s="7" t="n">
         <v>2003</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -9559,7 +9566,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9567,17 +9574,17 @@
         <v>279</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>2003</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J2" s="7"/>
     </row>
@@ -9586,17 +9593,17 @@
         <v>279</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>2003</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J3" s="7"/>
     </row>
@@ -9605,17 +9612,17 @@
         <v>279</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>2003</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J4" s="7"/>
     </row>
@@ -9624,17 +9631,17 @@
         <v>279</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>2003</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J5" s="7"/>
     </row>
@@ -9643,17 +9650,17 @@
         <v>279</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>2002</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="J6" s="7"/>
     </row>
@@ -9662,17 +9669,17 @@
         <v>279</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>2002</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="J7" s="7"/>
     </row>
@@ -9681,23 +9688,23 @@
         <v>279</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>2001</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -9731,7 +9738,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -9740,7 +9747,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -9752,16 +9759,16 @@
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="F2" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -9773,16 +9780,16 @@
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F3" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -9794,16 +9801,16 @@
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -9815,16 +9822,16 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F5" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -9836,16 +9843,16 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>2021</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -9857,16 +9864,16 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>2018</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -9878,16 +9885,16 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F8" s="7" t="n">
         <v>2016</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -9899,16 +9906,16 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F9" s="7" t="n">
         <v>2016</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -9920,16 +9927,16 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>2016</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -9941,16 +9948,16 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F11" s="7" t="n">
         <v>2015</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -9962,7 +9969,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>271</v>
@@ -9971,7 +9978,7 @@
         <v>2015</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -9983,16 +9990,16 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F13" s="7" t="n">
         <v>2015</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -10001,7 +10008,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>274</v>
@@ -10010,241 +10017,241 @@
         <v>2015</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="7" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F15" s="7" t="n">
         <v>2015</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="7" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F16" s="7" t="n">
         <v>2013</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="7" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F17" s="7" t="n">
         <v>2013</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="7" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F18" s="7" t="n">
         <v>2013</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="7" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F19" s="7" t="n">
         <v>2013</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="7" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F20" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="7" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F21" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F22" s="7" t="n">
         <v>2012</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="7" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="F23" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="7" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="F24" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="7" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F25" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="7" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F26" s="7" t="n">
         <v>2011</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="7" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F27" s="7" t="n">
         <v>2010</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="7" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F28" s="7" t="n">
         <v>2010</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="7" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F29" s="7" t="n">
         <v>2010</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="7" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F30" s="7" t="n">
         <v>2009</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -10282,19 +10289,19 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -10303,14 +10310,14 @@
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="7" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H2" s="7" t="n">
         <v>2018</v>
@@ -10319,14 +10326,14 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="7" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>2018</v>
@@ -10335,158 +10342,158 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="7" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="7" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>564</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>565</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>563</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="7" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>570</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>571</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>569</v>
       </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="7" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="7" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="7" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="7" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H12" s="7" t="n">
         <v>2006</v>
@@ -10495,14 +10502,14 @@
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="7" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>2008</v>
@@ -10511,14 +10518,14 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>2005</v>
@@ -10569,25 +10576,25 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -10596,60 +10603,60 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="7" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="7" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="J3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>600</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>597</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>599</v>
       </c>
       <c r="J4" s="7"/>
     </row>
@@ -10659,16 +10666,16 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="J5" s="16" t="n">
         <v>215734</v>
@@ -10683,13 +10690,13 @@
         <v>132</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>605</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>604</v>
       </c>
       <c r="J6" s="16" t="n">
         <v>215734</v>
@@ -10697,20 +10704,20 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="7" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>2019</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="J7" s="16" t="n">
         <v>5000000</v>
@@ -10718,22 +10725,22 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>609</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>610</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>611</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>608</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="J8" s="16" t="n">
         <v>1488744</v>
@@ -10741,41 +10748,41 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="7" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="7" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="J10" s="16" t="n">
         <v>1860000</v>
@@ -10783,22 +10790,22 @@
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="7" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>622</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>621</v>
       </c>
       <c r="J11" s="16" t="n">
         <v>1860000</v>
@@ -10806,39 +10813,39 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="7" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="7" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>2008</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="J13" s="16" t="n">
         <v>1564735</v>
@@ -10846,14 +10853,14 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="7" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>2008</v>
@@ -10863,22 +10870,22 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="7" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H15" s="7" t="n">
         <v>2008</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="J15" s="17" t="n">
         <v>5387180</v>
@@ -10886,22 +10893,22 @@
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="7" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H16" s="7" t="n">
         <v>2008</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="J16" s="16" t="n">
         <v>937508</v>
@@ -10909,66 +10916,66 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="7" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="7" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="7" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H19" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J19" s="16" t="n">
         <v>3355031</v>
@@ -10976,22 +10983,22 @@
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="7" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="H20" s="7" t="n">
         <v>2004</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="J20" s="17" t="n">
         <v>880199</v>
@@ -10999,20 +11006,20 @@
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="7" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="J21" s="16" t="n">
         <v>3000</v>
@@ -11020,22 +11027,22 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="19" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="7" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="7" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en regex en la búsqueda del autor que irá en negrita
</commit_message>
<xml_diff>
--- a/Para.Ivan_Pagina web.xlsx
+++ b/Para.Ivan_Pagina web.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="714">
   <si>
     <t xml:space="preserve">g</t>
   </si>
@@ -840,7 +840,7 @@
     <t xml:space="preserve">more info</t>
   </si>
   <si>
-    <t xml:space="preserve">	Pierce, G.J., Gutiérrez, P., Fariñas, A., Fernández, D., Petitguyot, M., Read, F.L., Hernández, A., Saavedra, C., Hernandez-Milian, G., Viñas Diéguez, L., Pérez Fernández, B., Jaquot, S., Méndez, P., López, A. y Cedeira, J.</t>
+    <t xml:space="preserve">Pierce, G.J., Gutiérrez, P., Fariñas, A., Fernández, D., Petitguyot, M., Read, F.L., Hernández, A., Saavedra, C., Hernandez-Milian, G., Viñas Diéguez, L., Pérez Fernández, B., Jaquot, S., Méndez, P., López, A. y Cedeira, J.</t>
   </si>
   <si>
     <t xml:space="preserve">Impacts of organic pollutants on cetaceans in NW Spain</t>
@@ -1110,7 +1110,7 @@
     <t xml:space="preserve">https://www.researchgate.net/publication/360 160317_Relacion_entre_la_dieta_y_la_carga_parasitaria_en_el_delfin_comun_Delphinus_delphis_en_Galicia</t>
   </si>
   <si>
-    <t xml:space="preserve">	Fariñas, A., Gutiérrez, P., Gil, Á., Roumbedakis, K., Hernandez-Milian, G., Petitguyot, M., Álvarez, M., Saavedra, C., Hernández-González, A., Verutes, G., Rodríguez, R., Correia, A.M., Valeiras, J., Rotllant, J., Suárez-Bregua, P., García, M., Saborido-Rey, F., Rivera, M.L., Alonso, A. y Pierce, G.J.</t>
+    <t xml:space="preserve">Fariñas, A., Gutiérrez, P., Gil, Á., Roumbedakis, K., Hernandez-Milian, G., Petitguyot, M., Álvarez, M., Saavedra, C., Hernández-González, A., Verutes, G., Rodríguez, R., Correia, A.M., Valeiras, J., Rotllant, J., Suárez-Bregua, P., García, M., Saborido-Rey, F., Rivera, M.L., Alonso, A. y Pierce, G.J.</t>
   </si>
   <si>
     <t xml:space="preserve">Our waves in the ocean: Projects for marine conservation and sustainable fisheries</t>
@@ -3849,6 +3849,12 @@
   </si>
   <si>
     <t xml:space="preserve">Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Pierce, G.J., Gutiérrez, P., Fariñas, A., Fernández, D., Petitguyot, M., Read, F.L., Hernández, A., Saavedra, C., Hernandez-Milian, G., Viñas Diéguez, L., Pérez Fernández, B., Jaquot, S., Méndez, P., López, A. y Cedeira, J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Fariñas, A., Gutiérrez, P., Gil, Á., Roumbedakis, K., Hernandez-Milian, G., Petitguyot, M., Álvarez, M., Saavedra, C., Hernández-González, A., Verutes, G., Rodríguez, R., Correia, A.M., Valeiras, J., Rotllant, J., Suárez-Bregua, P., García, M., Saborido-Rey, F., Rivera, M.L., Alonso, A. y Pierce, G.J.</t>
   </si>
   <si>
     <t xml:space="preserve">Waiting RG request</t>
@@ -5667,7 +5673,7 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="7" t="s">
-        <v>166</v>
+        <v>710</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>167</v>
@@ -5817,7 +5823,7 @@
     </row>
     <row r="10" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="7" t="s">
-        <v>196</v>
+        <v>711</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>197</v>
@@ -6159,7 +6165,7 @@
     </row>
     <row r="26" s="7" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="21" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>262</v>
@@ -6600,7 +6606,7 @@
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="22"/>
       <c r="D47" s="7" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>324</v>
@@ -7459,8 +7465,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>